<commit_message>
nand / nor / xor
</commit_message>
<xml_diff>
--- a/wahrheitstabellen.xlsx
+++ b/wahrheitstabellen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\Desktop\01_Basic_Logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0171AC-83FB-488E-A7EA-4A32B24DFB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8BD97A-89E5-4E1E-B85A-90E8B6AE20DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47880" yWindow="0" windowWidth="9825" windowHeight="15585" activeTab="2" xr2:uid="{7401F6F3-C5AA-4CB9-BB5E-5D33022E5919}"/>
+    <workbookView xWindow="44760" yWindow="0" windowWidth="12945" windowHeight="15585" firstSheet="1" activeTab="5" xr2:uid="{7401F6F3-C5AA-4CB9-BB5E-5D33022E5919}"/>
   </bookViews>
   <sheets>
     <sheet name="AND" sheetId="1" r:id="rId1"/>
@@ -744,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA33BA60-9DFA-4E65-8DDB-DA154AAED40A}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -805,7 +805,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,7 +841,9 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="2" t="s">
@@ -853,7 +855,9 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
@@ -862,7 +866,9 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
@@ -871,7 +877,9 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:D7">
@@ -888,7 +896,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,7 +932,9 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="2" t="s">
@@ -936,7 +946,9 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
@@ -945,7 +957,9 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
@@ -954,7 +968,9 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:D7">
@@ -970,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C066902-8C64-4E34-BF61-6C3DA04D79C8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,7 +1023,9 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="2" t="s">
@@ -1019,7 +1037,9 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
@@ -1028,7 +1048,9 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
@@ -1037,7 +1059,9 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:D7">

</xml_diff>